<commit_message>
TestCase and Test Report Automation Testing updated
</commit_message>
<xml_diff>
--- a/doc/Project Assignment/PA05/TestReport_Group04.xlsx
+++ b/doc/Project Assignment/PA05/TestReport_Group04.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phy\Desktop\ThisSemester\SoftwareEngineering\PA5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phy\Documents\GitHub\cs300-assignment1\doc\Project Assignment\PA05\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Tester</t>
   </si>
@@ -101,24 +101,15 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>UC001</t>
-  </si>
-  <si>
     <t>28/5/2015</t>
   </si>
   <si>
-    <t>HTThanh, NKHuy</t>
-  </si>
-  <si>
     <t>Defect ID</t>
   </si>
   <si>
     <t>B001</t>
   </si>
   <si>
-    <t>B002</t>
-  </si>
-  <si>
     <t>Defect Title</t>
   </si>
   <si>
@@ -131,34 +122,28 @@
     <t>Date Reported</t>
   </si>
   <si>
-    <t>Unable to login with correct username and password</t>
-  </si>
-  <si>
-    <t>System does not allow to login even with correct username and passwords</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Incorrect lable for login button</t>
-  </si>
-  <si>
-    <t>The label should be "Đăng Nhập" for the login button in the login page instead of "Đăng nhap"</t>
-  </si>
-  <si>
     <t>Open</t>
   </si>
   <si>
-    <t>Closed</t>
-  </si>
-  <si>
     <t>Reported By</t>
   </si>
   <si>
-    <t>Vu Nguyen</t>
-  </si>
-  <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>TTThong,LTPhy</t>
+  </si>
+  <si>
+    <t>S-FS-01</t>
+  </si>
+  <si>
+    <t>The description and caption do not appear as expected in sharing window</t>
+  </si>
+  <si>
+    <t>Phy Lieng</t>
+  </si>
+  <si>
+    <t>The description and caption do not appear as expected in sharing window since the app have not availabe on store yet.</t>
   </si>
 </sst>
 </file>
@@ -231,6 +216,40 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -252,45 +271,11 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="12"/>
+      <tableStyleElement type="headerRow" dxfId="11"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -305,17 +290,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I9" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I8" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <tableColumns count="9">
-    <tableColumn id="1" name="Defect ID" dataDxfId="10"/>
-    <tableColumn id="3" name="Defect Title" dataDxfId="9"/>
-    <tableColumn id="11" name="Defect Description" dataDxfId="8"/>
-    <tableColumn id="10" name="Function ID" dataDxfId="7"/>
-    <tableColumn id="5" name="Severity" dataDxfId="6"/>
-    <tableColumn id="12" name="Reported By" dataDxfId="5"/>
-    <tableColumn id="6" name="Date Reported" dataDxfId="4"/>
-    <tableColumn id="8" name="Status" dataDxfId="3"/>
-    <tableColumn id="9" name="Comment" dataDxfId="2"/>
+    <tableColumn id="1" name="Defect ID" dataDxfId="8"/>
+    <tableColumn id="3" name="Defect Title" dataDxfId="7"/>
+    <tableColumn id="11" name="Defect Description" dataDxfId="6"/>
+    <tableColumn id="10" name="Function ID" dataDxfId="5"/>
+    <tableColumn id="5" name="Severity" dataDxfId="4"/>
+    <tableColumn id="12" name="Reported By" dataDxfId="3"/>
+    <tableColumn id="6" name="Date Reported" dataDxfId="2"/>
+    <tableColumn id="8" name="Status" dataDxfId="1"/>
+    <tableColumn id="9" name="Comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -645,7 +630,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -675,7 +660,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -694,10 +679,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,25 +703,25 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
@@ -745,57 +730,34 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G2" s="7">
-        <v>42149</v>
+        <v>43086</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="7">
-        <v>42149</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G4" s="7"/>
@@ -811,9 +773,6 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change TestPlan + Test Report summary
</commit_message>
<xml_diff>
--- a/doc/Project Assignment/PA05/TestReport_Group04.xlsx
+++ b/doc/Project Assignment/PA05/TestReport_Group04.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Test summary report" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Tester</t>
   </si>
@@ -144,6 +144,39 @@
   </si>
   <si>
     <t>The description and caption do not appear as expected in sharing window since the app have not availabe on store yet.</t>
+  </si>
+  <si>
+    <t>Function be Tested</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> number of test cases</t>
+  </si>
+  <si>
+    <t>number of passed test cases,</t>
+  </si>
+  <si>
+    <t>number of failed test cases of a function</t>
+  </si>
+  <si>
+    <t>Function 01: Load Data and Create a List Of Object in Scroll View</t>
+  </si>
+  <si>
+    <t>Function 02: Switch Between Lists</t>
+  </si>
+  <si>
+    <t>Function 03: Click Item and Load Buy View</t>
+  </si>
+  <si>
+    <t>Function 04: Load Item Information in Buy View</t>
+  </si>
+  <si>
+    <t>Function 05: Quantity View</t>
+  </si>
+  <si>
+    <t>Function 06: Facebook Sharing</t>
+  </si>
+  <si>
+    <t>Function 07: Progress Tracking</t>
   </si>
 </sst>
 </file>
@@ -627,16 +660,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
     <col min="4" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" customWidth="1"/>
@@ -669,7 +703,60 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
       <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -681,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>